<commit_message>
VAI VAI VAI VAAAI
</commit_message>
<xml_diff>
--- a/SPRINT2/Planilha Backlog.xlsx
+++ b/SPRINT2/Planilha Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Desktop\Bandtec\TECCHICKEN-SPRINT2\SPRINT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosec\OneDrive\Documentos\Arquivos PI\Grupo 10\TECCHICKEN\SPRINT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{824A7B75-9DDE-485B-81CF-A95090A8D058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F55C1A-C46C-421F-BA5F-DC8E2BBF8849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{25395986-EBD6-45E1-B5FA-D5805360109E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="598" xr2:uid="{25395986-EBD6-45E1-B5FA-D5805360109E}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -182,6 +173,9 @@
   </si>
   <si>
     <t>Site Estático Cadastro e Login - Local</t>
+  </si>
+  <si>
+    <t>Script do Banco de Dados</t>
   </si>
 </sst>
 </file>
@@ -666,7 +660,7 @@
   <dimension ref="B1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +888,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13" s="13">
         <v>5</v>
@@ -912,7 +906,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="13">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E14" s="13">
         <v>6</v>
@@ -980,7 +974,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="7">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7">
         <v>8</v>
@@ -993,11 +987,11 @@
       <c r="B19" s="13">
         <v>8</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>47</v>
+      <c r="C19" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D19" s="7">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E19" s="7">
         <v>9</v>
@@ -1011,23 +1005,31 @@
         <v>9</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="7">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E20" s="7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="13">
+        <v>10</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="7">
+        <v>13</v>
+      </c>
+      <c r="E21" s="7">
+        <v>7</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>

</xml_diff>

<commit_message>
n sei oq ele vai enviar
</commit_message>
<xml_diff>
--- a/SPRINT2/Planilha Backlog.xlsx
+++ b/SPRINT2/Planilha Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42371d61bd3278c/Área de Trabalho/Sprint 3/TECCHICKEN-DOCUMENTACAO/SPRINT2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="13_ncr:1_{2D4F4366-4475-4FF2-B7AD-F1421C615BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08C0131E-BE9D-4583-944E-122CD663FA51}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{7B5D4B23-C96A-4D4B-BAE2-38923F007648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25395986-EBD6-45E1-B5FA-D5805360109E}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Requisitos" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -210,12 +211,6 @@
     <t>1, 2, 3</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Projeto criado e configurado no GitHub</t>
   </si>
   <si>
@@ -244,9 +239,6 @@
   </si>
   <si>
     <t>Escolher e testar o sensor no simulador</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>Planilha de riscos do projeto</t>
@@ -539,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -621,9 +613,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -643,9 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -661,39 +647,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -831,6 +796,12 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -861,7 +832,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95158068-8EBD-4465-A987-ECEB2A1FCD50}" name="Tabela32" displayName="Tabela32" ref="A42:E49" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95158068-8EBD-4465-A987-ECEB2A1FCD50}" name="Tabela32" displayName="Tabela32" ref="A42:E49" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A42:E49" xr:uid="{95158068-8EBD-4465-A987-ECEB2A1FCD50}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:D49">
     <sortCondition ref="A42:A49"/>
@@ -878,30 +849,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B062C9D8-73C4-46EB-B059-DAA54D1E0B94}" name="Tabela325" displayName="Tabela325" ref="A1:E40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
-  <autoFilter ref="A1:E40" xr:uid="{B062C9D8-73C4-46EB-B059-DAA54D1E0B94}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
-    <sortCondition ref="A4294967288:A4294967295"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD04FE12-824F-4F35-84C0-D755E422C462}" name="Tabela2" displayName="Tabela2" ref="B2:F19" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9A45F353-9CFD-4C78-BD5A-066735C2EA01}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{0252D482-772B-45B3-9870-374B93399D35}" name="Requisitos" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C0557B63-625D-42FF-BE9E-D8D8CCD9F3C6}" name="Tamanho" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BF5CA4B4-063A-4630-B5E5-1FC6866EC54C}" name="Ordem de Execução" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E8965E4E-B682-4858-A350-988D1ECD5701}" name="Sprint" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD04FE12-824F-4F35-84C0-D755E422C462}" name="Tabela2" displayName="Tabela2" ref="B2:F19" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7E8AE91F-6B94-4572-B2C8-99E2BD645D54}" name="ID" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{7E8AE91F-6B94-4572-B2C8-99E2BD645D54}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{FC7518A0-1AD6-468E-992C-47CC3022333D}" name="Requisitos"/>
-    <tableColumn id="3" xr3:uid="{D6E45C21-4863-40C2-BCFC-0EC4BA16E0DE}" name="Tamanho" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{BB463502-3145-4DB6-B84E-42F29CC5AB92}" name="Ordem de Execução" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{20485B11-2A81-4338-AD53-E3131C57B67A}" name="Sprint" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{D6E45C21-4863-40C2-BCFC-0EC4BA16E0DE}" name="Tamanho" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{BB463502-3145-4DB6-B84E-42F29CC5AB92}" name="Ordem de Execução" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{20485B11-2A81-4338-AD53-E3131C57B67A}" name="Sprint" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1207,7 +1161,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,19 +1192,19 @@
       <c r="G1">
         <v>1</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="44" t="s">
+      <c r="L1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="42" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1270,19 +1224,19 @@
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="K2" s="30">
-        <v>1</v>
-      </c>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="29">
+        <v>1</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="30">
         <v>21</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="30">
         <v>1</v>
       </c>
     </row>
@@ -1303,19 +1257,19 @@
         <f>G2+G1</f>
         <v>3</v>
       </c>
-      <c r="K3" s="32">
-        <v>2</v>
-      </c>
-      <c r="L3" s="33" t="s">
+      <c r="K3" s="31">
+        <v>2</v>
+      </c>
+      <c r="L3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="32">
         <v>16</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="32">
         <v>2</v>
       </c>
     </row>
@@ -1336,19 +1290,19 @@
         <f>G3+G2</f>
         <v>5</v>
       </c>
-      <c r="K4" s="30">
-        <v>3</v>
-      </c>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="29">
+        <v>3</v>
+      </c>
+      <c r="L4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="30">
         <v>18</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="30">
         <v>3</v>
       </c>
     </row>
@@ -1369,19 +1323,19 @@
         <f>G4+G3</f>
         <v>8</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="31">
         <v>4</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="32">
         <v>21</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="32">
         <v>4</v>
       </c>
     </row>
@@ -1402,19 +1356,19 @@
         <f>G5+G4</f>
         <v>13</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="29">
         <v>5</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="31">
-        <v>8</v>
-      </c>
-      <c r="O6" s="31">
+      <c r="N6" s="30">
+        <v>8</v>
+      </c>
+      <c r="O6" s="30">
         <v>5</v>
       </c>
     </row>
@@ -1435,19 +1389,19 @@
         <f>G6+G5</f>
         <v>21</v>
       </c>
-      <c r="K7" s="32">
+      <c r="K7" s="31">
         <v>6</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="L7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="32">
         <v>16</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="32">
         <v>6</v>
       </c>
     </row>
@@ -1464,70 +1418,70 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>7</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="30">
         <v>21</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="30">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K9" s="32">
-        <v>8</v>
-      </c>
-      <c r="L9" s="33" t="s">
+      <c r="K9" s="31">
+        <v>8</v>
+      </c>
+      <c r="L9" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="33">
-        <v>8</v>
-      </c>
-      <c r="O9" s="33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K10" s="30">
+      <c r="N9" s="32">
+        <v>8</v>
+      </c>
+      <c r="O9" s="32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="29">
         <v>9</v>
       </c>
-      <c r="L10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="31" t="s">
+      <c r="L10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="30">
         <v>13</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="30">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K11" s="32">
+      <c r="K11" s="31">
         <v>10</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="L11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="33">
-        <v>3</v>
-      </c>
-      <c r="O11" s="33">
+      <c r="N11" s="32">
+        <v>3</v>
+      </c>
+      <c r="O11" s="32">
         <v>10</v>
       </c>
     </row>
@@ -1543,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3685E5-F92C-42F0-8A9F-7AEF9F5411D3}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E49" sqref="A42:E49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E40" sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,680 +1515,680 @@
     <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:5" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <v>1</v>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="36">
+        <v>1</v>
+      </c>
+      <c r="D2" s="36">
+        <v>3</v>
+      </c>
+      <c r="E2" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>2</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="36">
+        <v>8</v>
+      </c>
+      <c r="D3" s="36">
+        <v>2</v>
+      </c>
+      <c r="E3" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <v>3</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="36">
+        <v>8</v>
+      </c>
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+      <c r="E4" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>4</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="37">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37">
-        <v>3</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
-        <v>2</v>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="C5" s="36">
+        <v>5</v>
+      </c>
+      <c r="D5" s="36">
+        <v>4</v>
+      </c>
+      <c r="E5" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>5</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="37">
-        <v>8</v>
-      </c>
-      <c r="D3" s="37">
-        <v>2</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
-        <v>3</v>
-      </c>
-      <c r="B4" s="38" t="s">
+      <c r="C6" s="36">
+        <v>13</v>
+      </c>
+      <c r="D6" s="36">
+        <v>9</v>
+      </c>
+      <c r="E6" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>6</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="36">
+        <v>21</v>
+      </c>
+      <c r="D7" s="36">
+        <v>10</v>
+      </c>
+      <c r="E7" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>7</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="36">
+        <v>8</v>
+      </c>
+      <c r="D8" s="36">
+        <v>5</v>
+      </c>
+      <c r="E8" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <v>8</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="36">
+        <v>5</v>
+      </c>
+      <c r="D9" s="36">
+        <v>6</v>
+      </c>
+      <c r="E9" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
+        <v>9</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="36">
+        <v>2</v>
+      </c>
+      <c r="D10" s="36">
+        <v>7</v>
+      </c>
+      <c r="E10" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>10</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="36">
+        <v>2</v>
+      </c>
+      <c r="D11" s="36">
+        <v>8</v>
+      </c>
+      <c r="E11" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <v>11</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="36">
+        <v>13</v>
+      </c>
+      <c r="D12" s="36">
+        <v>12</v>
+      </c>
+      <c r="E12" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>12</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="36">
+        <v>5</v>
+      </c>
+      <c r="D13" s="36">
+        <v>11</v>
+      </c>
+      <c r="E13" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="36">
+        <v>13</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="36">
+        <v>3</v>
+      </c>
+      <c r="D15" s="36">
+        <v>2</v>
+      </c>
+      <c r="E15" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <v>14</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="36">
+        <v>21</v>
+      </c>
+      <c r="D16" s="36">
+        <v>7</v>
+      </c>
+      <c r="E16" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="36">
+        <v>15</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="36">
+        <v>21</v>
+      </c>
+      <c r="D17" s="36">
+        <v>9</v>
+      </c>
+      <c r="E17" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>16</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="36">
+        <v>13</v>
+      </c>
+      <c r="D18" s="36">
+        <v>8</v>
+      </c>
+      <c r="E18" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="36">
+        <v>17</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="36">
+        <v>3</v>
+      </c>
+      <c r="D19" s="36">
+        <v>1</v>
+      </c>
+      <c r="E19" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="36">
+        <v>18</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="36">
+        <v>13</v>
+      </c>
+      <c r="D20" s="36">
+        <v>4</v>
+      </c>
+      <c r="E20" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>19</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="36">
+        <v>5</v>
+      </c>
+      <c r="D21" s="36">
+        <v>3</v>
+      </c>
+      <c r="E21" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
+        <v>20</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="36">
+        <v>8</v>
+      </c>
+      <c r="D22" s="36">
+        <v>5</v>
+      </c>
+      <c r="E22" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="36">
+        <v>21</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="36">
+        <v>5</v>
+      </c>
+      <c r="D23" s="36">
+        <v>6</v>
+      </c>
+      <c r="E23" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="36">
+        <v>22</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="36">
+        <v>13</v>
+      </c>
+      <c r="D24" s="36">
+        <v>11</v>
+      </c>
+      <c r="E24" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="36">
+        <v>23</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="36">
+        <v>8</v>
+      </c>
+      <c r="D25" s="36">
+        <v>10</v>
+      </c>
+      <c r="E25" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="36">
+        <v>24</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="36">
+        <v>3</v>
+      </c>
+      <c r="D27" s="36">
+        <v>12</v>
+      </c>
+      <c r="E27" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="36">
+        <v>25</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="36">
+        <v>13</v>
+      </c>
+      <c r="D28" s="36">
+        <v>13</v>
+      </c>
+      <c r="E28" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="36">
+        <v>26</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="36">
+        <v>8</v>
+      </c>
+      <c r="D29" s="36">
+        <v>14</v>
+      </c>
+      <c r="E29" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="36">
+        <v>27</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="36">
+        <v>8</v>
+      </c>
+      <c r="D30" s="36">
+        <v>11</v>
+      </c>
+      <c r="E30" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="36">
+        <v>28</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="36">
+        <v>21</v>
+      </c>
+      <c r="D31" s="36">
+        <v>8</v>
+      </c>
+      <c r="E31" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="36">
+        <v>29</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="36">
+        <v>21</v>
+      </c>
+      <c r="D32" s="36">
+        <v>6</v>
+      </c>
+      <c r="E32" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="36">
+        <v>30</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="36">
+        <v>8</v>
+      </c>
+      <c r="D33" s="36">
+        <v>7</v>
+      </c>
+      <c r="E33" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="36">
+        <v>31</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="36">
+        <v>13</v>
+      </c>
+      <c r="D34" s="36">
+        <v>4</v>
+      </c>
+      <c r="E34" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="36">
+        <v>32</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="36">
+        <v>5</v>
+      </c>
+      <c r="D35" s="36">
+        <v>5</v>
+      </c>
+      <c r="E35" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="36">
+        <v>8</v>
+      </c>
+      <c r="D36" s="36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="36">
+        <v>34</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="36">
+        <v>3</v>
+      </c>
+      <c r="D37" s="36">
+        <v>3</v>
+      </c>
+      <c r="E37" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="36">
+        <v>35</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="36">
+        <v>3</v>
+      </c>
+      <c r="D38" s="36">
+        <v>2</v>
+      </c>
+      <c r="E38" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="36">
         <v>36</v>
       </c>
-      <c r="C4" s="37">
-        <v>8</v>
-      </c>
-      <c r="D4" s="37">
-        <v>1</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
-        <v>4</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="37">
-        <v>5</v>
-      </c>
-      <c r="D5" s="37">
-        <v>4</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
-        <v>5</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="37">
+      <c r="B39" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="36">
+        <v>8</v>
+      </c>
+      <c r="D39" s="36">
+        <v>9</v>
+      </c>
+      <c r="E39" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="36">
+        <v>37</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="36">
         <v>13</v>
       </c>
-      <c r="D6" s="37">
-        <v>9</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
-        <v>6</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="37">
-        <v>21</v>
-      </c>
-      <c r="D7" s="37">
+      <c r="D40" s="36">
         <v>10</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
-        <v>7</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="37">
-        <v>8</v>
-      </c>
-      <c r="D8" s="37">
-        <v>5</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
-        <v>8</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="37">
-        <v>5</v>
-      </c>
-      <c r="D9" s="37">
-        <v>6</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
-        <v>9</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="37">
-        <v>2</v>
-      </c>
-      <c r="D10" s="37">
-        <v>7</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
-        <v>10</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="37">
-        <v>2</v>
-      </c>
-      <c r="D11" s="37">
-        <v>8</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
-        <v>11</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="37">
-        <v>13</v>
-      </c>
-      <c r="D12" s="37">
-        <v>12</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="37">
-        <v>12</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="37">
-        <v>5</v>
-      </c>
-      <c r="D13" s="37">
-        <v>11</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="42"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
-        <v>13</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="37">
-        <v>3</v>
-      </c>
-      <c r="D15" s="37">
-        <v>2</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
-        <v>14</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="37">
-        <v>21</v>
-      </c>
-      <c r="D16" s="37">
-        <v>7</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37">
-        <v>15</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="37">
-        <v>21</v>
-      </c>
-      <c r="D17" s="37">
-        <v>9</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="37">
-        <v>16</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="37">
-        <v>13</v>
-      </c>
-      <c r="D18" s="37">
-        <v>8</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="37">
-        <v>17</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="37">
-        <v>3</v>
-      </c>
-      <c r="D19" s="37">
-        <v>1</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="37">
-        <v>18</v>
-      </c>
-      <c r="B20" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="37">
-        <v>13</v>
-      </c>
-      <c r="D20" s="37">
-        <v>4</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="37">
-        <v>19</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="37">
-        <v>5</v>
-      </c>
-      <c r="D21" s="37">
-        <v>3</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="37">
-        <v>20</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="37">
-        <v>8</v>
-      </c>
-      <c r="D22" s="37">
-        <v>5</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37">
-        <v>21</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="37">
-        <v>5</v>
-      </c>
-      <c r="D23" s="37">
-        <v>6</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="37">
-        <v>22</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="37">
-        <v>13</v>
-      </c>
-      <c r="D24" s="37">
-        <v>11</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
-        <v>23</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="37">
-        <v>8</v>
-      </c>
-      <c r="D25" s="37">
-        <v>10</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="42"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="37">
-        <v>24</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="37">
-        <v>3</v>
-      </c>
-      <c r="D27" s="37">
-        <v>12</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37">
-        <v>25</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="37">
-        <v>13</v>
-      </c>
-      <c r="D28" s="37">
-        <v>13</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37">
-        <v>26</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="37">
-        <v>8</v>
-      </c>
-      <c r="D29" s="37">
-        <v>14</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="37">
-        <v>27</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="37">
-        <v>8</v>
-      </c>
-      <c r="D30" s="37">
-        <v>11</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="37">
-        <v>28</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="37">
-        <v>21</v>
-      </c>
-      <c r="D31" s="37">
-        <v>8</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="37">
-        <v>29</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="37">
-        <v>21</v>
-      </c>
-      <c r="D32" s="37">
-        <v>6</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="37">
-        <v>30</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="37">
-        <v>8</v>
-      </c>
-      <c r="D33" s="37">
-        <v>7</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="37">
-        <v>31</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="37">
-        <v>13</v>
-      </c>
-      <c r="D34" s="37">
-        <v>4</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="37">
-        <v>32</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="37">
-        <v>5</v>
-      </c>
-      <c r="D35" s="37">
-        <v>5</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
-        <v>33</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="37">
-        <v>8</v>
-      </c>
-      <c r="D36" s="37">
-        <v>1</v>
-      </c>
-      <c r="E36" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="37">
-        <v>34</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="37">
-        <v>3</v>
-      </c>
-      <c r="D37" s="37">
-        <v>3</v>
-      </c>
-      <c r="E37" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="37">
-        <v>35</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="37">
-        <v>3</v>
-      </c>
-      <c r="D38" s="37">
-        <v>2</v>
-      </c>
-      <c r="E38" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="37">
-        <v>36</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="37">
-        <v>8</v>
-      </c>
-      <c r="D39" s="37">
-        <v>9</v>
-      </c>
-      <c r="E39" s="39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="37">
-        <v>37</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="37">
-        <v>13</v>
-      </c>
-      <c r="D40" s="37">
-        <v>10</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>57</v>
+      <c r="E40" s="44">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="35" t="s">
+      <c r="B42" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="34" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2251,7 +2205,7 @@
       <c r="D43">
         <v>4</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2268,7 +2222,7 @@
       <c r="D44">
         <v>5</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2285,7 +2239,7 @@
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="33" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2302,8 +2256,8 @@
       <c r="D46">
         <v>6</v>
       </c>
-      <c r="E46" s="34" t="s">
-        <v>57</v>
+      <c r="E46" s="45">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2319,8 +2273,8 @@
       <c r="D47">
         <v>7</v>
       </c>
-      <c r="E47" s="34" t="s">
-        <v>57</v>
+      <c r="E47" s="45">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2336,7 +2290,7 @@
       <c r="D48">
         <v>3</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2353,15 +2307,14 @@
       <c r="D49">
         <v>2</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="33" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2370,9 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DFE211-9289-4CE5-BEDB-9EB311B8F419}">
   <dimension ref="B1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2388,10 +2339,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">

</xml_diff>